<commit_message>
corporate policy Approver completed
</commit_message>
<xml_diff>
--- a/testdata/Excel data.xlsx
+++ b/testdata/Excel data.xlsx
@@ -3,15 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Self Booking Tools\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10590" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="8400" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Division" sheetId="4" r:id="rId4"/>
+    <sheet name="username" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J19"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>username</t>
   </si>
@@ -81,6 +88,87 @@
   </si>
   <si>
     <t>Password@12</t>
+  </si>
+  <si>
+    <t>Travellername</t>
+  </si>
+  <si>
+    <t>Kanchan</t>
+  </si>
+  <si>
+    <t>Dnata@2018</t>
+  </si>
+  <si>
+    <t>Ashish.k@dnata.com</t>
+  </si>
+  <si>
+    <t>TripType</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Bombay</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>dubai</t>
+  </si>
+  <si>
+    <t>china</t>
+  </si>
+  <si>
+    <t>europe</t>
+  </si>
+  <si>
+    <t>russia</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>Sapna.chopra@quadlabs.com</t>
+  </si>
+  <si>
+    <t>anurag.upadhyay@quadlabs.com</t>
+  </si>
+  <si>
+    <t>Sanjip.Yadav@quadlabs.com</t>
+  </si>
+  <si>
+    <t>Selvaraj.Ramasamy@bmw.in</t>
+  </si>
+  <si>
+    <t>Vinodh-Kumar.Sankaran@bmw.in</t>
+  </si>
+  <si>
+    <t>Niraj.Kumar@bmw.in</t>
+  </si>
+  <si>
+    <t>ashish.k@india.hrgworldwide.com</t>
+  </si>
+  <si>
+    <t>Approver 1</t>
+  </si>
+  <si>
+    <t>Approver 2</t>
+  </si>
+  <si>
+    <t>Approver 3</t>
+  </si>
+  <si>
+    <t>Test Test</t>
+  </si>
+  <si>
+    <t>No of Approver</t>
+  </si>
+  <si>
+    <t>sanjip yadav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saurabh Yadav </t>
   </si>
 </sst>
 </file>
@@ -442,118 +530,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="abhishek05882@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="Sapna.chopra@quadlabs.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>43490</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>43491</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -561,39 +721,342 @@
       <c r="I2" s="1">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43490</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43490</v>
+      </c>
+      <c r="G4" s="5">
+        <v>43491</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5">
+        <v>43490</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
code comitted for policy approver and corporate mangement
</commit_message>
<xml_diff>
--- a/testdata/Excel data.xlsx
+++ b/testdata/Excel data.xlsx
@@ -9,14 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="8400" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13830" windowHeight="5145" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Division" sheetId="4" r:id="rId4"/>
-    <sheet name="username" sheetId="5" r:id="rId5"/>
+    <sheet name="Branch" sheetId="6" r:id="rId3"/>
+    <sheet name="Department" sheetId="7" r:id="rId4"/>
+    <sheet name="Designation" sheetId="8" r:id="rId5"/>
+    <sheet name="EmployeeGrade" sheetId="9" r:id="rId6"/>
+    <sheet name="Passportvisaalert" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
+    <sheet name="Division" sheetId="4" r:id="rId9"/>
+    <sheet name="username" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
   <si>
     <t>username</t>
   </si>
@@ -169,6 +174,126 @@
   </si>
   <si>
     <t xml:space="preserve">Saurabh Yadav </t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>Contactname</t>
+  </si>
+  <si>
+    <t>ContactEmailAdresss</t>
+  </si>
+  <si>
+    <t>ContactMobile</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Branchemail</t>
+  </si>
+  <si>
+    <t>branchname</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>anurag upadhyay</t>
+  </si>
+  <si>
+    <t>haryana</t>
+  </si>
+  <si>
+    <t>gurgaon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">720 b jmd megapolis </t>
+  </si>
+  <si>
+    <t>qa@quadlabs.com</t>
+  </si>
+  <si>
+    <t>DELHI</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Departmentname</t>
+  </si>
+  <si>
+    <t>DepartmentEmail</t>
+  </si>
+  <si>
+    <t>DepartmentPhone</t>
+  </si>
+  <si>
+    <t>DepartmentFax</t>
+  </si>
+  <si>
+    <t>TravelBudget</t>
+  </si>
+  <si>
+    <t>Noofstaff</t>
+  </si>
+  <si>
+    <t>Nooftraveller</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>finance@bmw.in</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Quality TestEngineer</t>
+  </si>
+  <si>
+    <t>Categorycode</t>
+  </si>
+  <si>
+    <t>Categoryname</t>
+  </si>
+  <si>
+    <t>Quad 586</t>
+  </si>
+  <si>
+    <t>qa engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Passportexpirationalert month</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> visaexpirationalert month</t>
   </si>
 </sst>
 </file>
@@ -585,11 +710,68 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -640,6 +822,300 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>9874651222</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2165165141</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9879846551</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="1">
+        <v>877545</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>500000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -959,104 +1435,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A1" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>